<commit_message>
nueva versión en camino
</commit_message>
<xml_diff>
--- a/01_data/base_maestra_ids.xlsx
+++ b/01_data/base_maestra_ids.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="568">
   <si>
     <t>ID</t>
   </si>
@@ -28,6 +28,234 @@
     <t>ID_Visible</t>
   </si>
   <si>
+    <t>226315.1015</t>
+  </si>
+  <si>
+    <t>226315.1005</t>
+  </si>
+  <si>
+    <t>226315.1085</t>
+  </si>
+  <si>
+    <t>226315.1095</t>
+  </si>
+  <si>
+    <t>226315.1105</t>
+  </si>
+  <si>
+    <t>226315.1115</t>
+  </si>
+  <si>
+    <t>224845.1870</t>
+  </si>
+  <si>
+    <t>224845.1779</t>
+  </si>
+  <si>
+    <t>225924.1032</t>
+  </si>
+  <si>
+    <t>225841.1522</t>
+  </si>
+  <si>
+    <t>224845.1234</t>
+  </si>
+  <si>
+    <t>225818.1264</t>
+  </si>
+  <si>
+    <t>225841.1871</t>
+  </si>
+  <si>
+    <t>225841.1373</t>
+  </si>
+  <si>
+    <t>225841.1459</t>
+  </si>
+  <si>
+    <t>225832.1036</t>
+  </si>
+  <si>
+    <t>225841.1616</t>
+  </si>
+  <si>
+    <t>225841.1431</t>
+  </si>
+  <si>
+    <t>224845.1567</t>
+  </si>
+  <si>
+    <t>225841.1475</t>
+  </si>
+  <si>
+    <t>225945.1003</t>
+  </si>
+  <si>
+    <t>224845.1643</t>
+  </si>
+  <si>
+    <t>225814.1119</t>
+  </si>
+  <si>
+    <t>225841.1600</t>
+  </si>
+  <si>
+    <t>225841.1586</t>
+  </si>
+  <si>
+    <t>225814.1078</t>
+  </si>
+  <si>
+    <t>224845.1536</t>
+  </si>
+  <si>
+    <t>224845.1028</t>
+  </si>
+  <si>
+    <t>225832.1115</t>
+  </si>
+  <si>
+    <t>225841.1505</t>
+  </si>
+  <si>
+    <t>225841.1723</t>
+  </si>
+  <si>
+    <t>225945.1011</t>
+  </si>
+  <si>
+    <t>225841.1554</t>
+  </si>
+  <si>
+    <t>225845.1033</t>
+  </si>
+  <si>
+    <t>225841.1855</t>
+  </si>
+  <si>
+    <t>224845.1041</t>
+  </si>
+  <si>
+    <t>225837.1038</t>
+  </si>
+  <si>
+    <t>225814.1046</t>
+  </si>
+  <si>
+    <t>225924.1019</t>
+  </si>
+  <si>
+    <t>225924.1009</t>
+  </si>
+  <si>
+    <t>224845.1372</t>
+  </si>
+  <si>
+    <t>225837.1056</t>
+  </si>
+  <si>
+    <t>225841.1403</t>
+  </si>
+  <si>
+    <t>225841.1356</t>
+  </si>
+  <si>
+    <t>225841.1385</t>
+  </si>
+  <si>
+    <t>225845.1020</t>
+  </si>
+  <si>
+    <t>225843.1048</t>
+  </si>
+  <si>
+    <t>225841.1840</t>
+  </si>
+  <si>
+    <t>225841.1693</t>
+  </si>
+  <si>
+    <t>225841.1415</t>
+  </si>
+  <si>
+    <t>225832.1077</t>
+  </si>
+  <si>
+    <t>225841.1447</t>
+  </si>
+  <si>
+    <t>225841.1541</t>
+  </si>
+  <si>
+    <t>225818.1459</t>
+  </si>
+  <si>
+    <t>225236.1005</t>
+  </si>
+  <si>
+    <t>225236.1010</t>
+  </si>
+  <si>
+    <t>225841.1783</t>
+  </si>
+  <si>
+    <t>225841.1739</t>
+  </si>
+  <si>
+    <t>225841.1769</t>
+  </si>
+  <si>
+    <t>224845.1793</t>
+  </si>
+  <si>
+    <t>224845.1748</t>
+  </si>
+  <si>
+    <t>225837.1004</t>
+  </si>
+  <si>
+    <t>224845.1217</t>
+  </si>
+  <si>
+    <t>225837.1055</t>
+  </si>
+  <si>
+    <t>225814.1184</t>
+  </si>
+  <si>
+    <t>224845.1671</t>
+  </si>
+  <si>
+    <t>224845.1734</t>
+  </si>
+  <si>
+    <t>224845.1184</t>
+  </si>
+  <si>
+    <t>224845.1400</t>
+  </si>
+  <si>
+    <t>224845.1657</t>
+  </si>
+  <si>
+    <t>224845.1856</t>
+  </si>
+  <si>
+    <t>225832.1019</t>
+  </si>
+  <si>
+    <t>224845.1342</t>
+  </si>
+  <si>
+    <t>225814.1089</t>
+  </si>
+  <si>
+    <t>224845.1093</t>
+  </si>
+  <si>
+    <t>224845.1581</t>
+  </si>
+  <si>
     <t>225832.1049</t>
   </si>
   <si>
@@ -223,6 +451,234 @@
     <t>225629.1001</t>
   </si>
   <si>
+    <t>ENGLISH FOR LEARNING - 226315.1015 (Remoto)</t>
+  </si>
+  <si>
+    <t>ENGLISH FOR LEARNING - 226315.1005 (Remoto)</t>
+  </si>
+  <si>
+    <t>ENGLISH FOR LEARNING - 226315.1085 (Remoto)</t>
+  </si>
+  <si>
+    <t>ENGLISH FOR LEARNING - 226315.1095 (Remoto)</t>
+  </si>
+  <si>
+    <t>ENGLISH FOR LEARNING - 226315.1105 (Remoto)</t>
+  </si>
+  <si>
+    <t>ENGLISH FOR LEARNING - 226315.1115 (Remoto)</t>
+  </si>
+  <si>
+    <t>PROG. PRES. Y PRES. RESULTADOS - 224845.1870 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 224845.1779 (Remoto)</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN GEST. CAM. PUB. - 225924.1032 (Remoto)</t>
+  </si>
+  <si>
+    <t>SIST. DE GEST. DE SE.INF. - 225841.1522 (Presencial)</t>
+  </si>
+  <si>
+    <t>COACHING Y TRABAJO EN EQUIPO - 224845.1234 (Remoto)</t>
+  </si>
+  <si>
+    <t>GESTIÓN ÁGIL DE PROYECTOS - 225818.1264 (Presencial)</t>
+  </si>
+  <si>
+    <t>SALUD MENTAL PUB PERSPECT EPID - 225841.1871 (Remoto)</t>
+  </si>
+  <si>
+    <t>CICLO DE VIDA DEL IMPAC. AMBI. - 225841.1373 (Remoto)</t>
+  </si>
+  <si>
+    <t>PLANIF.Y CONTROL DE LA CONST. - 225841.1459 (Remoto)</t>
+  </si>
+  <si>
+    <t>MÓDULO DE INVESTIGACIÓN - 225832.1036 (Remoto)</t>
+  </si>
+  <si>
+    <t>FILOSOFÍA LEAN CONST - 225841.1616 (Remoto)</t>
+  </si>
+  <si>
+    <t>COACHING Y LIDERAZGO EDUCATIVO - 225841.1431 (Remoto)</t>
+  </si>
+  <si>
+    <t>GESTIÓN DE SERVICIOS DE TI - 224845.1567 (Remoto)</t>
+  </si>
+  <si>
+    <t>GESTIÓN DEL RRHH EN MINERÍA - 225841.1475 (Remoto)</t>
+  </si>
+  <si>
+    <t>DESARRO. SOSTE. Y POLIT. PUB. - 225945.1003 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 224845.1643 (Remoto)</t>
+  </si>
+  <si>
+    <t>MANAG. Y ESTRA. BIM - 225814.1119 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 225841.1600 (Remoto)</t>
+  </si>
+  <si>
+    <t>ANÁLISIS ECONÓMICO DE LOS IMP - 225841.1586 (Remoto)</t>
+  </si>
+  <si>
+    <t>MÓDULO DE INVESTIGACIÓN GCGPPM - 225814.1078 (Remoto)</t>
+  </si>
+  <si>
+    <t>PROC. DE RES. Y TRAN. DE CONF. - 224845.1536 (Remoto)</t>
+  </si>
+  <si>
+    <t>DERIVADOS FINANCIEROS - 224845.1028 (Presencial)</t>
+  </si>
+  <si>
+    <t>COORDINACIÓN DE PROY - 225832.1115 (Remoto)</t>
+  </si>
+  <si>
+    <t>INNOVACIÓN Y TRANSF. DIGITAL - 225841.1505 (Remoto)</t>
+  </si>
+  <si>
+    <t>LIDERAZGO DIRECTIVO - 225841.1723 (Presencial)</t>
+  </si>
+  <si>
+    <t>IA APLICADA CREACIÓN CONTEN - 225945.1011 (Remoto)</t>
+  </si>
+  <si>
+    <t>MEJORA PRODUCTIVIDAD CONST - 225841.1554 (Remoto)</t>
+  </si>
+  <si>
+    <t>SIST PRESUP PÚBLICO ESTADO - 225845.1033 (Remoto)</t>
+  </si>
+  <si>
+    <t>GESTIÓN CALIDAD NORMA ISO 9001 - 225841.1855 (Remoto)</t>
+  </si>
+  <si>
+    <t>NEG Y CONFLICTOS EN EL ESTADO - 224845.1041 (Presencial)</t>
+  </si>
+  <si>
+    <t>SIST.DE EVAL.DE LA CONFO.Y AUD - 225837.1038 (Remoto)</t>
+  </si>
+  <si>
+    <t>MÓDULO DE INVESTIGACIÓN GCGPPM - 225814.1046 (Remoto)</t>
+  </si>
+  <si>
+    <t>MODERNIZACIÓN Y E-GOVERNMENT - 225924.1019 (Remoto)</t>
+  </si>
+  <si>
+    <t>PROYECTO DE DISRUPCIÓN TEC - 225924.1009 (Remoto)</t>
+  </si>
+  <si>
+    <t>STORYTELLING Y VISUALIZACIÓN - 224845.1372 (Presencial)</t>
+  </si>
+  <si>
+    <t>GER. ESTRATÉGICA DE LA CALIDAD - 225837.1056 (Remoto)</t>
+  </si>
+  <si>
+    <t>LID. GEST. DE EQUIPOS DE PROY - 225841.1403 (Remoto)</t>
+  </si>
+  <si>
+    <t>COACHING Y LIDERAZGO EDUCATIVO - 225841.1356 (Remoto)</t>
+  </si>
+  <si>
+    <t>AGILIDAD ORGANIZACIONAL - 225841.1385 (Remoto)</t>
+  </si>
+  <si>
+    <t>GERENCIA ESTRAT DE LA CALIDAD - 225845.1020 (Remoto)</t>
+  </si>
+  <si>
+    <t>GESTIÓN ESTRATÉGICA EN INGEN. - 225843.1048 (Remoto)</t>
+  </si>
+  <si>
+    <t>NETWORKING CLOUD - 225841.1840 (Remoto)</t>
+  </si>
+  <si>
+    <t>COACHING ONTOLOGICO - 225841.1693 (Remoto)</t>
+  </si>
+  <si>
+    <t>FILOSOFÍA LEAN CONST - 225841.1415 (Presencial)</t>
+  </si>
+  <si>
+    <t>FILOSOFÍA LEAN CONST - 225832.1077 (Remoto)</t>
+  </si>
+  <si>
+    <t>FINANZAS CORPORATIVAS - 225841.1447 (Remoto)</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN ESTRATÉGICA DE COMUN - 225841.1541 (Remoto)</t>
+  </si>
+  <si>
+    <t>GEREN. PROY. INVERSIÓN SALUD - 225818.1459 (Remoto)</t>
+  </si>
+  <si>
+    <t>Dis Optim Cad Sum - 225236.1005 (Remoto)</t>
+  </si>
+  <si>
+    <t>Seminario Integrador - 225236.1010 (Remoto)</t>
+  </si>
+  <si>
+    <t>EPIDEMIOLOGÍA EN SECTOR SALUD - 225841.1783 (Presencial)</t>
+  </si>
+  <si>
+    <t>GESTIÓN DE PRECIOS - 225841.1739 (Remoto)</t>
+  </si>
+  <si>
+    <t>GES. PLANE. ESTRATÉGICO SALUD - 225841.1769 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 224845.1793 (Remoto)</t>
+  </si>
+  <si>
+    <t>COMP. PENAL CORP. - 224845.1748 (Remoto)</t>
+  </si>
+  <si>
+    <t>PLANEA Y PRESUP. PÚB.D. EST.P. - 225837.1004 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 224845.1217 (Remoto)</t>
+  </si>
+  <si>
+    <t>COMPLIANCE Y NEGOCIOS - 225837.1055 (Remoto)</t>
+  </si>
+  <si>
+    <t>MÓDULO DE INVESTIGACIÓN - 225814.1184 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 224845.1671 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 224845.1734 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 224845.1184 (Remoto)</t>
+  </si>
+  <si>
+    <t>EVA TRAT TRAST ALIMENT EMERG - 224845.1400 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 224845.1657 (Remoto)</t>
+  </si>
+  <si>
+    <t>CIUDAD. DESARROLLO SOSTENIBLE - 224845.1856 (Remoto)</t>
+  </si>
+  <si>
+    <t>ENFOQUES Y MODELOS - 225832.1019 (Remoto)</t>
+  </si>
+  <si>
+    <t>CONTRATACIÓN DE OBRAS - 224845.1342 (Remoto)</t>
+  </si>
+  <si>
+    <t>MÓDULO DE INVESTIGACIÓN - 225814.1089 (Remoto)</t>
+  </si>
+  <si>
+    <t>HERRAM Y APLIC CONT ELEC SEACE - 224845.1093 (Remoto)</t>
+  </si>
+  <si>
+    <t>INNOVA TECNOLÓGICA DISRUPTIVA - 224845.1581 (Remoto)</t>
+  </si>
+  <si>
     <t>EPIDEMIOLOGÍA CE - 225832.1049 (Remoto)</t>
   </si>
   <si>
@@ -418,6 +874,234 @@
     <t>PORTUGUÉS INTERMEDIO B1 - 225629.1001 (Remoto)</t>
   </si>
   <si>
+    <t>_1626799_1</t>
+  </si>
+  <si>
+    <t>_1626694_1</t>
+  </si>
+  <si>
+    <t>_1626196_1</t>
+  </si>
+  <si>
+    <t>_1626190_1</t>
+  </si>
+  <si>
+    <t>_1626178_1</t>
+  </si>
+  <si>
+    <t>_1626171_1</t>
+  </si>
+  <si>
+    <t>_1626139_1</t>
+  </si>
+  <si>
+    <t>_1626138_1</t>
+  </si>
+  <si>
+    <t>_1626137_1</t>
+  </si>
+  <si>
+    <t>_1626136_1</t>
+  </si>
+  <si>
+    <t>_1626135_1</t>
+  </si>
+  <si>
+    <t>_1626134_1</t>
+  </si>
+  <si>
+    <t>_1626133_1</t>
+  </si>
+  <si>
+    <t>_1626132_1</t>
+  </si>
+  <si>
+    <t>_1626131_1</t>
+  </si>
+  <si>
+    <t>_1626130_1</t>
+  </si>
+  <si>
+    <t>_1626129_1</t>
+  </si>
+  <si>
+    <t>_1626128_1</t>
+  </si>
+  <si>
+    <t>_1626127_1</t>
+  </si>
+  <si>
+    <t>_1626126_1</t>
+  </si>
+  <si>
+    <t>_1626125_1</t>
+  </si>
+  <si>
+    <t>_1626124_1</t>
+  </si>
+  <si>
+    <t>_1626123_1</t>
+  </si>
+  <si>
+    <t>_1626122_1</t>
+  </si>
+  <si>
+    <t>_1626121_1</t>
+  </si>
+  <si>
+    <t>_1626120_1</t>
+  </si>
+  <si>
+    <t>_1626119_1</t>
+  </si>
+  <si>
+    <t>_1626118_1</t>
+  </si>
+  <si>
+    <t>_1626117_1</t>
+  </si>
+  <si>
+    <t>_1626116_1</t>
+  </si>
+  <si>
+    <t>_1626115_1</t>
+  </si>
+  <si>
+    <t>_1626114_1</t>
+  </si>
+  <si>
+    <t>_1626113_1</t>
+  </si>
+  <si>
+    <t>_1626112_1</t>
+  </si>
+  <si>
+    <t>_1626111_1</t>
+  </si>
+  <si>
+    <t>_1626110_1</t>
+  </si>
+  <si>
+    <t>_1626109_1</t>
+  </si>
+  <si>
+    <t>_1626108_1</t>
+  </si>
+  <si>
+    <t>_1626107_1</t>
+  </si>
+  <si>
+    <t>_1626106_1</t>
+  </si>
+  <si>
+    <t>_1626105_1</t>
+  </si>
+  <si>
+    <t>_1626104_1</t>
+  </si>
+  <si>
+    <t>_1626103_1</t>
+  </si>
+  <si>
+    <t>_1626102_1</t>
+  </si>
+  <si>
+    <t>_1626101_1</t>
+  </si>
+  <si>
+    <t>_1626100_1</t>
+  </si>
+  <si>
+    <t>_1626099_1</t>
+  </si>
+  <si>
+    <t>_1626098_1</t>
+  </si>
+  <si>
+    <t>_1626097_1</t>
+  </si>
+  <si>
+    <t>_1626096_1</t>
+  </si>
+  <si>
+    <t>_1626095_1</t>
+  </si>
+  <si>
+    <t>_1626094_1</t>
+  </si>
+  <si>
+    <t>_1626093_1</t>
+  </si>
+  <si>
+    <t>_1624869_1</t>
+  </si>
+  <si>
+    <t>_1624868_1</t>
+  </si>
+  <si>
+    <t>_1624867_1</t>
+  </si>
+  <si>
+    <t>_1624865_1</t>
+  </si>
+  <si>
+    <t>_1624866_1</t>
+  </si>
+  <si>
+    <t>_1624864_1</t>
+  </si>
+  <si>
+    <t>_1624819_1</t>
+  </si>
+  <si>
+    <t>_1624818_1</t>
+  </si>
+  <si>
+    <t>_1624817_1</t>
+  </si>
+  <si>
+    <t>_1624816_1</t>
+  </si>
+  <si>
+    <t>_1624815_1</t>
+  </si>
+  <si>
+    <t>_1624814_1</t>
+  </si>
+  <si>
+    <t>_1624813_1</t>
+  </si>
+  <si>
+    <t>_1624812_1</t>
+  </si>
+  <si>
+    <t>_1624811_1</t>
+  </si>
+  <si>
+    <t>_1624810_1</t>
+  </si>
+  <si>
+    <t>_1624809_1</t>
+  </si>
+  <si>
+    <t>_1624808_1</t>
+  </si>
+  <si>
+    <t>_1624807_1</t>
+  </si>
+  <si>
+    <t>_1624805_1</t>
+  </si>
+  <si>
+    <t>_1624806_1</t>
+  </si>
+  <si>
+    <t>_1624804_1</t>
+  </si>
+  <si>
+    <t>_1624803_1</t>
+  </si>
+  <si>
     <t>_1624788_1</t>
   </si>
   <si>
@@ -611,6 +1295,234 @@
   </si>
   <si>
     <t>_1603824_1</t>
+  </si>
+  <si>
+    <t>IDIO.0010.226315.1015.R</t>
+  </si>
+  <si>
+    <t>IDIO.0010.226315.1005.R</t>
+  </si>
+  <si>
+    <t>IDIO.0010.226315.1085.R</t>
+  </si>
+  <si>
+    <t>IDIO.0010.226315.1095.R</t>
+  </si>
+  <si>
+    <t>IDIO.0010.226315.1105.R</t>
+  </si>
+  <si>
+    <t>IDIO.0010.226315.1115.R</t>
+  </si>
+  <si>
+    <t>FINN.5134.224845.1870.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.224845.1779.R</t>
+  </si>
+  <si>
+    <t>MARK.6147.225924.1032.R</t>
+  </si>
+  <si>
+    <t>ITEC.5118.225841.1522.P</t>
+  </si>
+  <si>
+    <t>RRHH.5110.224845.1234.R</t>
+  </si>
+  <si>
+    <t>MAGM.5177.225818.1264.P</t>
+  </si>
+  <si>
+    <t>MAGM.5230.225841.1871.R</t>
+  </si>
+  <si>
+    <t>IAMB.5104.225841.1373.R</t>
+  </si>
+  <si>
+    <t>MAGM.5431.225841.1459.R</t>
+  </si>
+  <si>
+    <t>INVE.5236.225832.1036.R</t>
+  </si>
+  <si>
+    <t>MAGM.5213.225841.1616.R</t>
+  </si>
+  <si>
+    <t>RRHH.5129.225841.1431.R</t>
+  </si>
+  <si>
+    <t>ITEC.5123.224845.1567.R</t>
+  </si>
+  <si>
+    <t>MAGM.5184.225841.1475.R</t>
+  </si>
+  <si>
+    <t>MAGM.6106.225945.1003.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.224845.1643.R</t>
+  </si>
+  <si>
+    <t>MAGM.5215.225814.1119.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.225841.1600.R</t>
+  </si>
+  <si>
+    <t>ECON.5109.225841.1586.R</t>
+  </si>
+  <si>
+    <t>INVE.5018.225814.1078.R</t>
+  </si>
+  <si>
+    <t>MAGM.5294.224845.1536.R</t>
+  </si>
+  <si>
+    <t>FINN.6103.224845.1028.P</t>
+  </si>
+  <si>
+    <t>MAGM.5218.225832.1115.R</t>
+  </si>
+  <si>
+    <t>MAGM.5121.225841.1505.R</t>
+  </si>
+  <si>
+    <t>MAGM.5126.225841.1723.P</t>
+  </si>
+  <si>
+    <t>MARK.5165.225945.1011.R</t>
+  </si>
+  <si>
+    <t>MAGM.5212.225841.1554.R</t>
+  </si>
+  <si>
+    <t>MAGM.5232.225845.1033.R</t>
+  </si>
+  <si>
+    <t>MAGM.5135.225841.1855.R</t>
+  </si>
+  <si>
+    <t>MAGM.6186.224845.1041.P</t>
+  </si>
+  <si>
+    <t>MAGM.5148.225837.1038.R</t>
+  </si>
+  <si>
+    <t>INVE.5018.225814.1046.R</t>
+  </si>
+  <si>
+    <t>MAGM.6179.225924.1019.R</t>
+  </si>
+  <si>
+    <t>ITEC.6124.225924.1009.R</t>
+  </si>
+  <si>
+    <t>MAGM.5139.224845.1372.P</t>
+  </si>
+  <si>
+    <t>MAGM.5144.225837.1056.R</t>
+  </si>
+  <si>
+    <t>MAGM.5214.225841.1403.R</t>
+  </si>
+  <si>
+    <t>RRHH.5129.225841.1356.R</t>
+  </si>
+  <si>
+    <t>MAGM.5416.225841.1385.R</t>
+  </si>
+  <si>
+    <t>MAGM.5438.225845.1020.R</t>
+  </si>
+  <si>
+    <t>MAGM.5316.225843.1048.R</t>
+  </si>
+  <si>
+    <t>MAGM.5200.225841.1840.R</t>
+  </si>
+  <si>
+    <t>RRHH.5123.225841.1693.R</t>
+  </si>
+  <si>
+    <t>MAGM.5213.225841.1415.P</t>
+  </si>
+  <si>
+    <t>MAGM.5213.225832.1077.R</t>
+  </si>
+  <si>
+    <t>FINN.5127.225841.1447.R</t>
+  </si>
+  <si>
+    <t>MAGM.5124.225841.1541.R</t>
+  </si>
+  <si>
+    <t>MAGM.5280.225818.1459.R</t>
+  </si>
+  <si>
+    <t>MAGM.8047.225236.1005.R</t>
+  </si>
+  <si>
+    <t>PSGE.6122.225236.1010.R</t>
+  </si>
+  <si>
+    <t>MAGM.5277.225841.1783.P</t>
+  </si>
+  <si>
+    <t>MARK.5143.225841.1739.R</t>
+  </si>
+  <si>
+    <t>MAGM.5276.225841.1769.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.224845.1793.R</t>
+  </si>
+  <si>
+    <t>DEPR.5117.224845.1748.R</t>
+  </si>
+  <si>
+    <t>MAGM.5348.225837.1004.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.224845.1217.R</t>
+  </si>
+  <si>
+    <t>MAGM.5143.225837.1055.R</t>
+  </si>
+  <si>
+    <t>INVE.5236.225814.1184.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.224845.1671.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.224845.1734.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.224845.1184.R</t>
+  </si>
+  <si>
+    <t>PSGE.5109.224845.1400.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.224845.1657.R</t>
+  </si>
+  <si>
+    <t>MAGM.5181.224845.1856.R</t>
+  </si>
+  <si>
+    <t>MAGM.5273.225832.1019.R</t>
+  </si>
+  <si>
+    <t>MAGM.5239.224845.1342.R</t>
+  </si>
+  <si>
+    <t>INVE.5236.225814.1089.R</t>
+  </si>
+  <si>
+    <t>MAGM.5296.224845.1093.R</t>
+  </si>
+  <si>
+    <t>ITEC.5124.224845.1581.R</t>
   </si>
   <si>
     <t>PSCL.5001.225832.1049.R</t>
@@ -1167,7 +2079,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1198,13 +2110,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>286</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1212,13 +2124,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>287</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1226,13 +2138,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>288</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1240,13 +2152,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>289</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1254,13 +2166,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>290</v>
       </c>
       <c r="D6" t="s">
-        <v>203</v>
+        <v>431</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1268,13 +2180,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>291</v>
       </c>
       <c r="D7" t="s">
-        <v>204</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1282,13 +2194,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>292</v>
       </c>
       <c r="D8" t="s">
-        <v>205</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1296,13 +2208,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>293</v>
       </c>
       <c r="D9" t="s">
-        <v>206</v>
+        <v>434</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1310,13 +2222,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>294</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>435</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1324,13 +2236,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>154</v>
       </c>
       <c r="C11" t="s">
-        <v>143</v>
+        <v>295</v>
       </c>
       <c r="D11" t="s">
-        <v>208</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1338,13 +2250,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>155</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>296</v>
       </c>
       <c r="D12" t="s">
-        <v>209</v>
+        <v>437</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1352,13 +2264,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>297</v>
       </c>
       <c r="D13" t="s">
-        <v>210</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1366,13 +2278,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>298</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>439</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1380,13 +2292,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>299</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1394,13 +2306,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>148</v>
+        <v>300</v>
       </c>
       <c r="D16" t="s">
-        <v>213</v>
+        <v>441</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1408,13 +2320,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>301</v>
       </c>
       <c r="D17" t="s">
-        <v>214</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1422,13 +2334,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>302</v>
       </c>
       <c r="D18" t="s">
-        <v>215</v>
+        <v>443</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1436,13 +2348,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>303</v>
       </c>
       <c r="D19" t="s">
-        <v>216</v>
+        <v>444</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1450,13 +2362,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>163</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>304</v>
       </c>
       <c r="D20" t="s">
-        <v>217</v>
+        <v>445</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1464,13 +2376,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
+        <v>305</v>
       </c>
       <c r="D21" t="s">
-        <v>218</v>
+        <v>446</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1478,13 +2390,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>306</v>
       </c>
       <c r="D22" t="s">
-        <v>219</v>
+        <v>447</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1492,13 +2404,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
+        <v>307</v>
       </c>
       <c r="D23" t="s">
-        <v>220</v>
+        <v>448</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1506,13 +2418,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>167</v>
       </c>
       <c r="C24" t="s">
-        <v>156</v>
+        <v>308</v>
       </c>
       <c r="D24" t="s">
-        <v>221</v>
+        <v>449</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1520,13 +2432,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
+        <v>309</v>
       </c>
       <c r="D25" t="s">
-        <v>222</v>
+        <v>450</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1534,13 +2446,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>169</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>310</v>
       </c>
       <c r="D26" t="s">
-        <v>223</v>
+        <v>451</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1548,13 +2460,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>170</v>
       </c>
       <c r="C27" t="s">
-        <v>159</v>
+        <v>311</v>
       </c>
       <c r="D27" t="s">
-        <v>224</v>
+        <v>452</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1562,13 +2474,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>171</v>
       </c>
       <c r="C28" t="s">
-        <v>160</v>
+        <v>312</v>
       </c>
       <c r="D28" t="s">
-        <v>225</v>
+        <v>453</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1576,13 +2488,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
+        <v>313</v>
       </c>
       <c r="D29" t="s">
-        <v>226</v>
+        <v>454</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1590,13 +2502,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="C30" t="s">
-        <v>162</v>
+        <v>314</v>
       </c>
       <c r="D30" t="s">
-        <v>227</v>
+        <v>455</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1604,13 +2516,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>174</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
+        <v>315</v>
       </c>
       <c r="D31" t="s">
-        <v>228</v>
+        <v>456</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1618,13 +2530,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>175</v>
       </c>
       <c r="C32" t="s">
-        <v>164</v>
+        <v>316</v>
       </c>
       <c r="D32" t="s">
-        <v>229</v>
+        <v>457</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1632,13 +2544,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
+        <v>317</v>
       </c>
       <c r="D33" t="s">
-        <v>230</v>
+        <v>458</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1646,13 +2558,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>177</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
+        <v>318</v>
       </c>
       <c r="D34" t="s">
-        <v>231</v>
+        <v>459</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1660,13 +2572,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
       <c r="C35" t="s">
-        <v>167</v>
+        <v>319</v>
       </c>
       <c r="D35" t="s">
-        <v>232</v>
+        <v>460</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1674,13 +2586,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>179</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
+        <v>320</v>
       </c>
       <c r="D36" t="s">
-        <v>233</v>
+        <v>461</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1688,13 +2600,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>180</v>
       </c>
       <c r="C37" t="s">
-        <v>169</v>
+        <v>321</v>
       </c>
       <c r="D37" t="s">
-        <v>234</v>
+        <v>462</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1702,13 +2614,13 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="C38" t="s">
-        <v>170</v>
+        <v>322</v>
       </c>
       <c r="D38" t="s">
-        <v>235</v>
+        <v>463</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1716,13 +2628,13 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>182</v>
       </c>
       <c r="C39" t="s">
-        <v>171</v>
+        <v>323</v>
       </c>
       <c r="D39" t="s">
-        <v>236</v>
+        <v>464</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1730,13 +2642,13 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>183</v>
       </c>
       <c r="C40" t="s">
-        <v>172</v>
+        <v>324</v>
       </c>
       <c r="D40" t="s">
-        <v>237</v>
+        <v>465</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1744,13 +2656,13 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="C41" t="s">
-        <v>173</v>
+        <v>325</v>
       </c>
       <c r="D41" t="s">
-        <v>238</v>
+        <v>466</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1758,13 +2670,13 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>185</v>
       </c>
       <c r="C42" t="s">
-        <v>174</v>
+        <v>326</v>
       </c>
       <c r="D42" t="s">
-        <v>239</v>
+        <v>467</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1772,13 +2684,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>186</v>
       </c>
       <c r="C43" t="s">
-        <v>175</v>
+        <v>327</v>
       </c>
       <c r="D43" t="s">
-        <v>240</v>
+        <v>468</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1786,13 +2698,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>187</v>
       </c>
       <c r="C44" t="s">
-        <v>176</v>
+        <v>328</v>
       </c>
       <c r="D44" t="s">
-        <v>241</v>
+        <v>469</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1800,13 +2712,13 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>188</v>
       </c>
       <c r="C45" t="s">
-        <v>177</v>
+        <v>329</v>
       </c>
       <c r="D45" t="s">
-        <v>242</v>
+        <v>470</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1814,13 +2726,13 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>189</v>
       </c>
       <c r="C46" t="s">
-        <v>178</v>
+        <v>330</v>
       </c>
       <c r="D46" t="s">
-        <v>243</v>
+        <v>471</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1828,13 +2740,13 @@
         <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>190</v>
       </c>
       <c r="C47" t="s">
-        <v>179</v>
+        <v>331</v>
       </c>
       <c r="D47" t="s">
-        <v>244</v>
+        <v>472</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1842,13 +2754,13 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>191</v>
       </c>
       <c r="C48" t="s">
-        <v>180</v>
+        <v>332</v>
       </c>
       <c r="D48" t="s">
-        <v>245</v>
+        <v>473</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1856,13 +2768,13 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>192</v>
       </c>
       <c r="C49" t="s">
-        <v>181</v>
+        <v>333</v>
       </c>
       <c r="D49" t="s">
-        <v>246</v>
+        <v>474</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1870,13 +2782,13 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>193</v>
       </c>
       <c r="C50" t="s">
-        <v>182</v>
+        <v>334</v>
       </c>
       <c r="D50" t="s">
-        <v>247</v>
+        <v>475</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1884,13 +2796,13 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>194</v>
       </c>
       <c r="C51" t="s">
-        <v>183</v>
+        <v>335</v>
       </c>
       <c r="D51" t="s">
-        <v>248</v>
+        <v>476</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1898,13 +2810,13 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>195</v>
       </c>
       <c r="C52" t="s">
-        <v>184</v>
+        <v>336</v>
       </c>
       <c r="D52" t="s">
-        <v>249</v>
+        <v>477</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1912,13 +2824,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="C53" t="s">
-        <v>185</v>
+        <v>337</v>
       </c>
       <c r="D53" t="s">
-        <v>250</v>
+        <v>478</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1926,13 +2838,13 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>197</v>
       </c>
       <c r="C54" t="s">
-        <v>186</v>
+        <v>338</v>
       </c>
       <c r="D54" t="s">
-        <v>251</v>
+        <v>479</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1940,13 +2852,13 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>198</v>
       </c>
       <c r="C55" t="s">
-        <v>187</v>
+        <v>339</v>
       </c>
       <c r="D55" t="s">
-        <v>252</v>
+        <v>480</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1954,13 +2866,13 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>123</v>
+        <v>199</v>
       </c>
       <c r="C56" t="s">
-        <v>188</v>
+        <v>340</v>
       </c>
       <c r="D56" t="s">
-        <v>253</v>
+        <v>481</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1968,13 +2880,13 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>200</v>
       </c>
       <c r="C57" t="s">
-        <v>189</v>
+        <v>341</v>
       </c>
       <c r="D57" t="s">
-        <v>254</v>
+        <v>482</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1982,13 +2894,13 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>201</v>
       </c>
       <c r="C58" t="s">
-        <v>190</v>
+        <v>342</v>
       </c>
       <c r="D58" t="s">
-        <v>255</v>
+        <v>483</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1996,13 +2908,13 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>202</v>
       </c>
       <c r="C59" t="s">
-        <v>191</v>
+        <v>343</v>
       </c>
       <c r="D59" t="s">
-        <v>256</v>
+        <v>484</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2010,13 +2922,13 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>203</v>
       </c>
       <c r="C60" t="s">
-        <v>192</v>
+        <v>344</v>
       </c>
       <c r="D60" t="s">
-        <v>257</v>
+        <v>485</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2024,13 +2936,13 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>128</v>
+        <v>204</v>
       </c>
       <c r="C61" t="s">
-        <v>193</v>
+        <v>345</v>
       </c>
       <c r="D61" t="s">
-        <v>258</v>
+        <v>486</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2038,13 +2950,13 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>205</v>
       </c>
       <c r="C62" t="s">
-        <v>194</v>
+        <v>346</v>
       </c>
       <c r="D62" t="s">
-        <v>259</v>
+        <v>487</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2052,13 +2964,13 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>206</v>
       </c>
       <c r="C63" t="s">
-        <v>195</v>
+        <v>347</v>
       </c>
       <c r="D63" t="s">
-        <v>260</v>
+        <v>488</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2066,13 +2978,13 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>207</v>
       </c>
       <c r="C64" t="s">
-        <v>196</v>
+        <v>348</v>
       </c>
       <c r="D64" t="s">
-        <v>261</v>
+        <v>489</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2080,13 +2992,13 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>208</v>
       </c>
       <c r="C65" t="s">
-        <v>197</v>
+        <v>349</v>
       </c>
       <c r="D65" t="s">
-        <v>262</v>
+        <v>490</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2094,13 +3006,1077 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
+        <v>209</v>
+      </c>
+      <c r="C66" t="s">
+        <v>350</v>
+      </c>
+      <c r="D66" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" t="s">
+        <v>210</v>
+      </c>
+      <c r="C67" t="s">
+        <v>351</v>
+      </c>
+      <c r="D67" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" t="s">
+        <v>211</v>
+      </c>
+      <c r="C68" t="s">
+        <v>352</v>
+      </c>
+      <c r="D68" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" t="s">
+        <v>212</v>
+      </c>
+      <c r="C69" t="s">
+        <v>353</v>
+      </c>
+      <c r="D69" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" t="s">
+        <v>354</v>
+      </c>
+      <c r="D70" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" t="s">
+        <v>214</v>
+      </c>
+      <c r="C71" t="s">
+        <v>355</v>
+      </c>
+      <c r="D71" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" t="s">
+        <v>215</v>
+      </c>
+      <c r="C72" t="s">
+        <v>356</v>
+      </c>
+      <c r="D72" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" t="s">
+        <v>216</v>
+      </c>
+      <c r="C73" t="s">
+        <v>357</v>
+      </c>
+      <c r="D73" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" t="s">
+        <v>217</v>
+      </c>
+      <c r="C74" t="s">
+        <v>358</v>
+      </c>
+      <c r="D74" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" t="s">
+        <v>359</v>
+      </c>
+      <c r="D75" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" t="s">
+        <v>219</v>
+      </c>
+      <c r="C76" t="s">
+        <v>360</v>
+      </c>
+      <c r="D76" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" t="s">
+        <v>220</v>
+      </c>
+      <c r="C77" t="s">
+        <v>361</v>
+      </c>
+      <c r="D77" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" t="s">
+        <v>221</v>
+      </c>
+      <c r="C78" t="s">
+        <v>362</v>
+      </c>
+      <c r="D78" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" t="s">
+        <v>222</v>
+      </c>
+      <c r="C79" t="s">
+        <v>363</v>
+      </c>
+      <c r="D79" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" t="s">
+        <v>223</v>
+      </c>
+      <c r="C80" t="s">
+        <v>364</v>
+      </c>
+      <c r="D80" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B81" t="s">
+        <v>224</v>
+      </c>
+      <c r="C81" t="s">
+        <v>365</v>
+      </c>
+      <c r="D81" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" t="s">
+        <v>225</v>
+      </c>
+      <c r="C82" t="s">
+        <v>366</v>
+      </c>
+      <c r="D82" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" t="s">
+        <v>226</v>
+      </c>
+      <c r="C83" t="s">
+        <v>367</v>
+      </c>
+      <c r="D83" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>227</v>
+      </c>
+      <c r="C84" t="s">
+        <v>368</v>
+      </c>
+      <c r="D84" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" t="s">
+        <v>228</v>
+      </c>
+      <c r="C85" t="s">
+        <v>369</v>
+      </c>
+      <c r="D85" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" t="s">
+        <v>229</v>
+      </c>
+      <c r="C86" t="s">
+        <v>370</v>
+      </c>
+      <c r="D86" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B87" t="s">
+        <v>230</v>
+      </c>
+      <c r="C87" t="s">
+        <v>371</v>
+      </c>
+      <c r="D87" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" t="s">
+        <v>231</v>
+      </c>
+      <c r="C88" t="s">
+        <v>372</v>
+      </c>
+      <c r="D88" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" t="s">
+        <v>232</v>
+      </c>
+      <c r="C89" t="s">
+        <v>373</v>
+      </c>
+      <c r="D89" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" t="s">
+        <v>233</v>
+      </c>
+      <c r="C90" t="s">
+        <v>374</v>
+      </c>
+      <c r="D90" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91" t="s">
+        <v>234</v>
+      </c>
+      <c r="C91" t="s">
+        <v>375</v>
+      </c>
+      <c r="D91" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B92" t="s">
+        <v>235</v>
+      </c>
+      <c r="C92" t="s">
+        <v>376</v>
+      </c>
+      <c r="D92" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" t="s">
+        <v>236</v>
+      </c>
+      <c r="C93" t="s">
+        <v>377</v>
+      </c>
+      <c r="D93" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" t="s">
+        <v>237</v>
+      </c>
+      <c r="C94" t="s">
+        <v>378</v>
+      </c>
+      <c r="D94" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B95" t="s">
+        <v>238</v>
+      </c>
+      <c r="C95" t="s">
+        <v>379</v>
+      </c>
+      <c r="D95" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B96" t="s">
+        <v>239</v>
+      </c>
+      <c r="C96" t="s">
+        <v>380</v>
+      </c>
+      <c r="D96" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" t="s">
+        <v>240</v>
+      </c>
+      <c r="C97" t="s">
+        <v>381</v>
+      </c>
+      <c r="D97" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" t="s">
+        <v>241</v>
+      </c>
+      <c r="C98" t="s">
+        <v>382</v>
+      </c>
+      <c r="D98" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" t="s">
+        <v>242</v>
+      </c>
+      <c r="C99" t="s">
+        <v>383</v>
+      </c>
+      <c r="D99" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="s">
+        <v>243</v>
+      </c>
+      <c r="C100" t="s">
+        <v>384</v>
+      </c>
+      <c r="D100" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" t="s">
+        <v>244</v>
+      </c>
+      <c r="C101" t="s">
+        <v>385</v>
+      </c>
+      <c r="D101" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="s">
+        <v>245</v>
+      </c>
+      <c r="C102" t="s">
+        <v>386</v>
+      </c>
+      <c r="D102" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" t="s">
+        <v>246</v>
+      </c>
+      <c r="C103" t="s">
+        <v>387</v>
+      </c>
+      <c r="D103" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" t="s">
+        <v>247</v>
+      </c>
+      <c r="C104" t="s">
+        <v>388</v>
+      </c>
+      <c r="D104" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" t="s">
+        <v>248</v>
+      </c>
+      <c r="C105" t="s">
+        <v>389</v>
+      </c>
+      <c r="D105" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" t="s">
+        <v>249</v>
+      </c>
+      <c r="C106" t="s">
+        <v>390</v>
+      </c>
+      <c r="D106" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" t="s">
+        <v>250</v>
+      </c>
+      <c r="C107" t="s">
+        <v>391</v>
+      </c>
+      <c r="D107" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" t="s">
+        <v>251</v>
+      </c>
+      <c r="C108" t="s">
+        <v>392</v>
+      </c>
+      <c r="D108" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" t="s">
+        <v>252</v>
+      </c>
+      <c r="C109" t="s">
+        <v>393</v>
+      </c>
+      <c r="D109" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" t="s">
+        <v>253</v>
+      </c>
+      <c r="C110" t="s">
+        <v>394</v>
+      </c>
+      <c r="D110" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" t="s">
+        <v>254</v>
+      </c>
+      <c r="C111" t="s">
+        <v>395</v>
+      </c>
+      <c r="D111" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112" t="s">
+        <v>255</v>
+      </c>
+      <c r="C112" t="s">
+        <v>396</v>
+      </c>
+      <c r="D112" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B113" t="s">
+        <v>256</v>
+      </c>
+      <c r="C113" t="s">
+        <v>397</v>
+      </c>
+      <c r="D113" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B114" t="s">
+        <v>257</v>
+      </c>
+      <c r="C114" t="s">
+        <v>398</v>
+      </c>
+      <c r="D114" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B115" t="s">
+        <v>258</v>
+      </c>
+      <c r="C115" t="s">
+        <v>399</v>
+      </c>
+      <c r="D115" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116" t="s">
+        <v>259</v>
+      </c>
+      <c r="C116" t="s">
+        <v>400</v>
+      </c>
+      <c r="D116" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B117" t="s">
+        <v>260</v>
+      </c>
+      <c r="C117" t="s">
+        <v>401</v>
+      </c>
+      <c r="D117" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B118" t="s">
+        <v>261</v>
+      </c>
+      <c r="C118" t="s">
+        <v>402</v>
+      </c>
+      <c r="D118" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B119" t="s">
+        <v>262</v>
+      </c>
+      <c r="C119" t="s">
+        <v>403</v>
+      </c>
+      <c r="D119" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B120" t="s">
+        <v>263</v>
+      </c>
+      <c r="C120" t="s">
+        <v>404</v>
+      </c>
+      <c r="D120" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B121" t="s">
+        <v>264</v>
+      </c>
+      <c r="C121" t="s">
+        <v>405</v>
+      </c>
+      <c r="D121" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B122" t="s">
+        <v>265</v>
+      </c>
+      <c r="C122" t="s">
+        <v>406</v>
+      </c>
+      <c r="D122" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B123" t="s">
+        <v>266</v>
+      </c>
+      <c r="C123" t="s">
+        <v>407</v>
+      </c>
+      <c r="D123" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124" t="s">
+        <v>267</v>
+      </c>
+      <c r="C124" t="s">
+        <v>408</v>
+      </c>
+      <c r="D124" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" t="s">
+        <v>268</v>
+      </c>
+      <c r="C125" t="s">
+        <v>409</v>
+      </c>
+      <c r="D125" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B126" t="s">
+        <v>269</v>
+      </c>
+      <c r="C126" t="s">
+        <v>410</v>
+      </c>
+      <c r="D126" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B127" t="s">
+        <v>270</v>
+      </c>
+      <c r="C127" t="s">
+        <v>411</v>
+      </c>
+      <c r="D127" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B128" t="s">
+        <v>271</v>
+      </c>
+      <c r="C128" t="s">
+        <v>412</v>
+      </c>
+      <c r="D128" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B129" t="s">
+        <v>272</v>
+      </c>
+      <c r="C129" t="s">
+        <v>413</v>
+      </c>
+      <c r="D129" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130" t="s">
+        <v>273</v>
+      </c>
+      <c r="C130" t="s">
+        <v>414</v>
+      </c>
+      <c r="D130" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C66" t="s">
-        <v>198</v>
-      </c>
-      <c r="D66" t="s">
-        <v>263</v>
+      <c r="B131" t="s">
+        <v>274</v>
+      </c>
+      <c r="C131" t="s">
+        <v>415</v>
+      </c>
+      <c r="D131" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B132" t="s">
+        <v>275</v>
+      </c>
+      <c r="C132" t="s">
+        <v>416</v>
+      </c>
+      <c r="D132" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B133" t="s">
+        <v>276</v>
+      </c>
+      <c r="C133" t="s">
+        <v>417</v>
+      </c>
+      <c r="D133" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B134" t="s">
+        <v>277</v>
+      </c>
+      <c r="C134" t="s">
+        <v>418</v>
+      </c>
+      <c r="D134" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B135" t="s">
+        <v>278</v>
+      </c>
+      <c r="C135" t="s">
+        <v>419</v>
+      </c>
+      <c r="D135" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B136" t="s">
+        <v>279</v>
+      </c>
+      <c r="C136" t="s">
+        <v>420</v>
+      </c>
+      <c r="D136" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B137" t="s">
+        <v>280</v>
+      </c>
+      <c r="C137" t="s">
+        <v>421</v>
+      </c>
+      <c r="D137" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B138" t="s">
+        <v>281</v>
+      </c>
+      <c r="C138" t="s">
+        <v>422</v>
+      </c>
+      <c r="D138" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B139" t="s">
+        <v>282</v>
+      </c>
+      <c r="C139" t="s">
+        <v>423</v>
+      </c>
+      <c r="D139" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B140" t="s">
+        <v>283</v>
+      </c>
+      <c r="C140" t="s">
+        <v>424</v>
+      </c>
+      <c r="D140" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B141" t="s">
+        <v>284</v>
+      </c>
+      <c r="C141" t="s">
+        <v>425</v>
+      </c>
+      <c r="D141" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B142" t="s">
+        <v>285</v>
+      </c>
+      <c r="C142" t="s">
+        <v>426</v>
+      </c>
+      <c r="D142" t="s">
+        <v>567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>